<commit_message>
Final Test Case data
</commit_message>
<xml_diff>
--- a/data/test_case_2.xlsx
+++ b/data/test_case_2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Divya/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Divya/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9910AFEA-8008-0343-922B-E24606987283}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B0B5FF-A124-064C-BCD3-EFA65FB236B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7480" yWindow="500" windowWidth="27640" windowHeight="15900" xr2:uid="{90E76997-9A2C-E54E-80C7-0C05D2697DC5}"/>
+    <workbookView xWindow="3220" yWindow="500" windowWidth="27640" windowHeight="15900" xr2:uid="{90E76997-9A2C-E54E-80C7-0C05D2697DC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Country</t>
   </si>
@@ -45,24 +45,6 @@
     <t>R3</t>
   </si>
   <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>R20</t>
-  </si>
-  <si>
     <t>R21</t>
   </si>
   <si>
@@ -73,12 +55,6 @@
   </si>
   <si>
     <t>R24</t>
-  </si>
-  <si>
-    <t>R25</t>
-  </si>
-  <si>
-    <t>R26</t>
   </si>
   <si>
     <t>Brobdingnag</t>
@@ -97,7 +73,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -115,6 +91,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -152,10 +135,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -472,15 +456,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49FC575-B5EC-D945-AE10-3398C858E926}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="K1" sqref="K1:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -493,46 +477,22 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="B2">
         <v>35</v>
@@ -543,46 +503,22 @@
       <c r="D2">
         <v>15</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>20</v>
       </c>
-      <c r="F2">
-        <v>11</v>
-      </c>
-      <c r="G2">
-        <v>7</v>
-      </c>
-      <c r="H2">
+      <c r="F2" s="3">
+        <v>15</v>
+      </c>
+      <c r="G2" s="3">
         <v>40</v>
       </c>
-      <c r="I2">
-        <v>38</v>
-      </c>
-      <c r="J2">
-        <v>40</v>
-      </c>
-      <c r="K2">
-        <v>20</v>
-      </c>
-      <c r="L2">
-        <v>15</v>
-      </c>
-      <c r="M2">
-        <v>40</v>
-      </c>
-      <c r="N2">
+      <c r="H2" s="3">
         <v>10</v>
       </c>
-      <c r="O2">
-        <v>20</v>
-      </c>
-      <c r="P2">
-        <v>10</v>
-      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>40</v>
@@ -593,46 +529,22 @@
       <c r="D3">
         <v>20</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>15</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>15</v>
       </c>
-      <c r="G3">
-        <v>10</v>
-      </c>
-      <c r="H3">
+      <c r="G3" s="3">
         <v>45</v>
       </c>
-      <c r="I3">
-        <v>29</v>
-      </c>
-      <c r="J3">
-        <v>30</v>
-      </c>
-      <c r="K3">
-        <v>15</v>
-      </c>
-      <c r="L3">
-        <v>15</v>
-      </c>
-      <c r="M3">
-        <v>45</v>
-      </c>
-      <c r="N3">
+      <c r="H3" s="3">
         <v>20</v>
       </c>
-      <c r="O3">
-        <v>10</v>
-      </c>
-      <c r="P3">
-        <v>20</v>
-      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -643,46 +555,22 @@
       <c r="D4">
         <v>11</v>
       </c>
-      <c r="E4">
-        <v>11</v>
-      </c>
-      <c r="F4">
-        <v>11</v>
-      </c>
-      <c r="G4">
-        <v>8</v>
-      </c>
-      <c r="H4">
-        <v>30</v>
-      </c>
-      <c r="I4">
-        <v>11</v>
-      </c>
-      <c r="J4">
-        <v>5</v>
-      </c>
-      <c r="K4">
+      <c r="E4" s="3">
         <v>9</v>
       </c>
-      <c r="L4">
+      <c r="F4" s="3">
         <v>7</v>
       </c>
-      <c r="M4">
+      <c r="G4" s="3">
         <v>16</v>
       </c>
-      <c r="N4">
+      <c r="H4" s="3">
         <v>6</v>
       </c>
-      <c r="O4">
-        <v>3</v>
-      </c>
-      <c r="P4">
-        <v>5</v>
-      </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -693,41 +581,17 @@
       <c r="D5">
         <v>11</v>
       </c>
-      <c r="E5">
-        <v>7</v>
-      </c>
-      <c r="F5">
+      <c r="E5" s="3">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3">
+        <v>9</v>
+      </c>
+      <c r="G5" s="3">
         <v>8</v>
       </c>
-      <c r="G5">
-        <v>11</v>
-      </c>
-      <c r="H5">
-        <v>9</v>
-      </c>
-      <c r="I5">
-        <v>11</v>
-      </c>
-      <c r="J5">
-        <v>7</v>
-      </c>
-      <c r="K5">
-        <v>5</v>
-      </c>
-      <c r="L5">
-        <v>9</v>
-      </c>
-      <c r="M5">
+      <c r="H5" s="3">
         <v>8</v>
-      </c>
-      <c r="N5">
-        <v>8</v>
-      </c>
-      <c r="O5">
-        <v>5</v>
-      </c>
-      <c r="P5">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>